<commit_message>
incremental navigation self positioning text TextFormatting
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ref" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Navigation</t>
   </si>
   <si>
-    <t>Video Player</t>
-  </si>
-  <si>
     <t>more chaos in making videos work</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>Still rearranging various elements of old programming to accomidate different data approach, also reset the many aspects of the project files in general, like storage and versioning</t>
   </si>
   <si>
-    <t>Various</t>
-  </si>
-  <si>
     <t>Added new graphic changes, new "Action" section, Home Page images, reset positioning, change in logo etc.</t>
   </si>
   <si>
@@ -166,6 +160,63 @@
   </si>
   <si>
     <t>Refactored a lot of the framework so that it can handle a lot of different section layouts</t>
+  </si>
+  <si>
+    <t>April 18,2010</t>
+  </si>
+  <si>
+    <t>Training Package Framework/Manager</t>
+  </si>
+  <si>
+    <t>Test Framework/Manager</t>
+  </si>
+  <si>
+    <t>Shared Objects</t>
+  </si>
+  <si>
+    <t>Back End Data Collection</t>
+  </si>
+  <si>
+    <t>Dynamic Image Loader</t>
+  </si>
+  <si>
+    <t>Login/user registration</t>
+  </si>
+  <si>
+    <t>Subtitle Implementation</t>
+  </si>
+  <si>
+    <t>Text resizer</t>
+  </si>
+  <si>
+    <t>Screen Reading Capabilities</t>
+  </si>
+  <si>
+    <t>Configuration system</t>
+  </si>
+  <si>
+    <t>Graphics implementation</t>
+  </si>
+  <si>
+    <t>XML Loader/Data provider</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>TASK</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>XML Data Loader</t>
+  </si>
+  <si>
+    <t>Most work was actually in other areas but I'm pulling from this estimate to equalize hours. At this point the old estimate is nearly irrelevant as the project definition has changed drastically and the timeline has been completely blown out. Tasks completed were section continue navigation, video controls, and section text positioning / formatting.</t>
   </si>
 </sst>
 </file>
@@ -228,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +350,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -314,7 +371,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -369,6 +426,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -672,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -714,7 +778,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30">
@@ -858,7 +922,7 @@
         <v>142.5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="39" customHeight="1">
@@ -1050,10 +1114,10 @@
         <v>116.5</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1064,7 +1128,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2">
         <v>16</v>
@@ -1077,7 +1141,7 @@
         <v>111.5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30">
@@ -1101,7 +1165,7 @@
         <v>109.5</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1112,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="2">
         <v>10</v>
@@ -1125,12 +1189,12 @@
         <v>107.5</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="18" customFormat="1" ht="48" customHeight="1">
       <c r="A19" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="45">
@@ -1141,7 +1205,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="2">
         <v>10</v>
@@ -1153,7 +1217,7 @@
         <v>103.5</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1164,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="2">
         <v>20</v>
@@ -1176,7 +1240,7 @@
         <v>100.5</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="60">
@@ -1187,7 +1251,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="2">
         <v>20</v>
@@ -1199,7 +1263,7 @@
         <v>97.5</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30">
@@ -1210,7 +1274,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="2">
         <v>20</v>
@@ -1222,7 +1286,7 @@
         <v>94.5</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30">
@@ -1233,7 +1297,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D24" s="2">
         <v>10</v>
@@ -1245,7 +1309,7 @@
         <v>91.5</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30">
@@ -1255,7 +1319,7 @@
       <c r="B25" s="2">
         <v>4</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="2">
@@ -1268,7 +1332,7 @@
         <v>87.5</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30">
@@ -1278,7 +1342,7 @@
       <c r="B26" s="2">
         <v>4</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="2">
@@ -1291,7 +1355,30 @@
         <v>83.5</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="105">
+      <c r="A27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="2">
+        <v>9</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="2">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>74.5</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1305,13 +1392,264 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="41.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="19" customFormat="1" ht="23.25">
+      <c r="A1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <f>SUM(B2 - C2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D16" si="0">SUM(B3 - C3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>17.5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="23.25">
+      <c r="A16" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="19">
+        <f>SUM(B2:B15)</f>
+        <v>155</v>
+      </c>
+      <c r="C16" s="19">
+        <f>SUM(C2:C15)</f>
+        <v>80.5</v>
+      </c>
+      <c r="D16" s="19">
+        <f t="shared" si="0"/>
+        <v>74.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added new ImageCueLoader to handle a list of images with ids. The images are loaded sequentially, so that priority is given to the most likely to be viewed first.
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -421,18 +421,18 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1192,8 +1192,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="18" customFormat="1" ht="48" customHeight="1">
-      <c r="A19" s="17" t="s">
+    <row r="19" spans="1:7" s="21" customFormat="1" ht="48" customHeight="1">
+      <c r="A19" s="20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       <c r="B27" s="2">
         <v>9</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="19" t="s">
         <v>65</v>
       </c>
       <c r="D27" s="2">
@@ -1395,7 +1395,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1406,17 +1406,17 @@
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="19" customFormat="1" ht="23.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:4" s="17" customFormat="1" ht="23.25">
+      <c r="A1" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1503,11 +1503,11 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1630,21 +1630,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" ht="23.25">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:4" s="17" customFormat="1" ht="23.25">
+      <c r="A16" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="17">
         <f>SUM(B2:B15)</f>
         <v>155</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="17">
         <f>SUM(C2:C15)</f>
-        <v>80.5</v>
-      </c>
-      <c r="D16" s="19">
-        <f t="shared" si="0"/>
-        <v>74.5</v>
+        <v>83.5</v>
+      </c>
+      <c r="D16" s="17">
+        <f t="shared" si="0"/>
+        <v>71.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wired up ImageLoader... able to grab and display images from the section mediator by id
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>April 22,2010</t>
+  </si>
+  <si>
+    <t>Scroller</t>
+  </si>
+  <si>
+    <t>Image Loader Framework</t>
   </si>
 </sst>
 </file>
@@ -739,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F34" sqref="E34:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -1404,6 +1410,46 @@
         <v>71.5</v>
       </c>
     </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="6">
+        <v>40293</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10">
+        <v>-4</v>
+      </c>
+      <c r="F29" s="2">
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="6">
+        <v>40293</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>-2</v>
+      </c>
+      <c r="F30" s="2">
+        <v>63.5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:XFD19"/>
@@ -1418,7 +1464,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1481,11 +1527,11 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1511,11 +1557,11 @@
         <v>20</v>
       </c>
       <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
         <v>9</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1526,11 +1572,11 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1663,11 +1709,11 @@
       </c>
       <c r="C16" s="17">
         <f>SUM(C2:C15)</f>
-        <v>83.5</v>
+        <v>91.5</v>
       </c>
       <c r="D16" s="17">
         <f t="shared" si="0"/>
-        <v>71.5</v>
+        <v>63.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Image swamping on scroll
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>Image Loader Framework</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>More or less worked on the image switching mechanism. Using Configuration pool, as that was also affected by these changes. i.e. Only certain sections are configured to swamp images</t>
   </si>
 </sst>
 </file>
@@ -745,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F34" sqref="E34:F34"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -1450,6 +1456,29 @@
         <v>63.5</v>
       </c>
     </row>
+    <row r="31" spans="1:7" ht="60">
+      <c r="A31" s="6">
+        <v>40299</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="2">
+        <v>16</v>
+      </c>
+      <c r="E31" s="2">
+        <v>12</v>
+      </c>
+      <c r="F31" s="2">
+        <v>59.5</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:XFD19"/>
@@ -1464,7 +1493,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1662,11 +1691,11 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1709,11 +1738,11 @@
       </c>
       <c r="C16" s="17">
         <f>SUM(C2:C15)</f>
-        <v>91.5</v>
+        <v>95.5</v>
       </c>
       <c r="D16" s="17">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>59.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Cuepoint manager, used specified seconds to dispatch cuepoints. Added Action section and toolkit section. extracted Section content from SectionMediator into a SectionManager to handle all the branching paths for specialized sections. Able to create sections in the editor
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -766,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="34" spans="1:7" ht="60">
       <c r="A34" s="6">
-        <v>38869</v>
+        <v>40335</v>
       </c>
       <c r="B34" s="2">
         <v>8</v>
@@ -1561,6 +1561,46 @@
       </c>
       <c r="G34" s="1" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="6">
+        <v>40336</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>-18</v>
+      </c>
+      <c r="F35" s="2">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="6">
+        <v>40348</v>
+      </c>
+      <c r="B36" s="2">
+        <v>10</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>-28</v>
+      </c>
+      <c r="F36" s="2">
+        <v>27.5</v>
       </c>
     </row>
   </sheetData>
@@ -1576,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1820,11 +1860,11 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="17" customFormat="1" ht="23.25">
@@ -1837,11 +1877,11 @@
       </c>
       <c r="C17" s="17">
         <f>SUM(C2:C16)</f>
-        <v>115.5</v>
+        <v>127.5</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>39.5</v>
+        <v>27.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearranged and refactored content to better adapt to the customized sections. Added new Managers to handle media, custom sections and sequences. Created a baseclass for custom sections to maintain some consistency with the wildness of the project.
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -766,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -1603,6 +1603,26 @@
         <v>27.5</v>
       </c>
     </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="6">
+        <v>40349</v>
+      </c>
+      <c r="B37" s="2">
+        <v>8</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>-36</v>
+      </c>
+      <c r="F37" s="2">
+        <v>19.5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:XFD19"/>
@@ -1616,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1860,11 +1880,11 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>-20</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="17" customFormat="1" ht="23.25">
@@ -1877,11 +1897,11 @@
       </c>
       <c r="C17" s="17">
         <f>SUM(C2:C16)</f>
-        <v>127.5</v>
+        <v>135.5</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>27.5</v>
+        <v>19.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Direction for image loading
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -766,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -1621,6 +1621,26 @@
       </c>
       <c r="F37" s="2">
         <v>19.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="6">
+        <v>40350</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2">
+        <v>-37.5</v>
+      </c>
+      <c r="F38" s="2">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished loading scheme... all loaded at startup. Added rotating buffer and Loading Images label.
Still haven't reworked the access withing the project, however it is self-explainatory
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>More of the same described above. From now on, I will no longer specifically itemize work. Everything is a mish mash, and I will simply move the content forward until there are no hours left</t>
+  </si>
+  <si>
+    <t>Verious</t>
   </si>
 </sst>
 </file>
@@ -766,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -1643,6 +1646,26 @@
         <v>18</v>
       </c>
     </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="6">
+        <v>40351</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2">
+        <v>-38.5</v>
+      </c>
+      <c r="F39" s="2">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:XFD19"/>
@@ -1656,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1900,11 +1923,11 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>28</v>
+        <v>30.5</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>-28</v>
+        <v>-30.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="17" customFormat="1" ht="23.25">
@@ -1917,11 +1940,11 @@
       </c>
       <c r="C17" s="17">
         <f>SUM(C2:C16)</f>
-        <v>135.5</v>
+        <v>138</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>19.5</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added all section classes both visual and logic Completed layout of Remarkable Servivce Employee sections.
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Verious</t>
+  </si>
+  <si>
+    <t>June 23 2010</t>
   </si>
 </sst>
 </file>
@@ -769,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -1666,6 +1669,26 @@
         <v>17</v>
       </c>
     </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
+        <v>-39.5</v>
+      </c>
+      <c r="F40" s="2">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:XFD19"/>
@@ -1679,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1923,11 +1946,11 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>30.5</v>
+        <v>31.5</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>-30.5</v>
+        <v>-31.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="17" customFormat="1" ht="23.25">
@@ -1940,11 +1963,11 @@
       </c>
       <c r="C17" s="17">
         <f>SUM(C2:C16)</f>
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Most of the navigation complete Inserted hooks to all the image points Inserted event mechanism to signal section complete fixed sequential progress to run correctly.
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>June 23 2010</t>
+  </si>
+  <si>
+    <t>June 24 2010</t>
   </si>
 </sst>
 </file>
@@ -772,9 +775,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
@@ -1689,6 +1692,26 @@
         <v>16</v>
       </c>
     </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="2">
+        <v>10</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2">
+        <v>-49.5</v>
+      </c>
+      <c r="F41" s="2">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:XFD19"/>
@@ -1702,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1946,11 +1969,11 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>31.5</v>
+        <v>41.5</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>-31.5</v>
+        <v>-41.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="17" customFormat="1" ht="23.25">
@@ -1963,11 +1986,11 @@
       </c>
       <c r="C17" s="17">
         <f>SUM(C2:C16)</f>
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All ghostmonk obfuscated Placed into External SWC
</commit_message>
<xml_diff>
--- a/docs/GBC-hours.xlsx
+++ b/docs/GBC-hours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>June 24 2010</t>
+  </si>
+  <si>
+    <t>June 26 2010</t>
+  </si>
+  <si>
+    <t>various</t>
   </si>
 </sst>
 </file>
@@ -775,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -1712,6 +1718,26 @@
         <v>6</v>
       </c>
     </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="2">
+        <v>12</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <v>-61.5</v>
+      </c>
+      <c r="F42" s="2">
+        <v>-6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:XFD19"/>
@@ -1725,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1969,11 +1995,11 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>41.5</v>
+        <v>53.5</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>-41.5</v>
+        <v>-53.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="17" customFormat="1" ht="23.25">
@@ -1986,11 +2012,11 @@
       </c>
       <c r="C17" s="17">
         <f>SUM(C2:C16)</f>
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>